<commit_message>
Automatic commit, 2023-05-20 14:56:41.538209
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filiptomanka/Programming/excel_coding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programming\excel_coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BC01F2-09BC-2344-9F44-59ED8BF03264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4E8273-8DFA-4DED-893B-EE82F73A4534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="700" windowWidth="26740" windowHeight="16260" xr2:uid="{3BAF7A37-CF33-CA41-B834-014DE83E4310}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{3BAF7A37-CF33-CA41-B834-014DE83E4310}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>column1</t>
   </si>
@@ -453,24 +453,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45AE6EA-E293-8345-99F6-0C06C81533FA}">
-  <dimension ref="A1:CQ3260"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I28:I32"/>
+    <sheetView tabSelected="1" topLeftCell="CA3234" workbookViewId="0">
+      <selection activeCell="CM3242" sqref="CM3242"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" s="3"/>
       <c r="E4">
         <v>43142</v>
@@ -479,13 +479,13 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -506,7 +506,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>1</v>
       </c>
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>2</v>
       </c>
@@ -543,7 +543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>3</v>
       </c>
@@ -563,7 +563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>4</v>
       </c>
@@ -577,7 +577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>5</v>
       </c>
@@ -591,28 +591,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
       <c r="G14">
         <v>3141</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15" s="3"/>
       <c r="G15">
         <v>314134</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="3"/>
       <c r="K16">
         <v>43142</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
       <c r="G17">
         <v>431434312</v>
@@ -624,7 +624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D18" s="3"/>
       <c r="G18">
         <v>34113</v>
@@ -636,7 +636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D19" s="3"/>
       <c r="N19" t="s">
         <v>13</v>
@@ -645,7 +645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>0</v>
       </c>
@@ -659,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>1</v>
       </c>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>2</v>
       </c>
@@ -687,7 +687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>3</v>
       </c>
@@ -707,7 +707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>4</v>
       </c>
@@ -727,7 +727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>5</v>
       </c>
@@ -747,7 +747,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="N26" t="s">
         <v>14</v>
@@ -756,69 +756,37 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
       <c r="I28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
       <c r="I29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
       <c r="I30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="I31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D32" s="3"/>
       <c r="I32" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3257" spans="94:95" x14ac:dyDescent="0.2">
-      <c r="CP3257" t="s">
-        <v>10</v>
-      </c>
-      <c r="CQ3257" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3258" spans="94:95" x14ac:dyDescent="0.2">
-      <c r="CP3258" t="s">
-        <v>12</v>
-      </c>
-      <c r="CQ3258">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3259" spans="94:95" x14ac:dyDescent="0.2">
-      <c r="CP3259" t="s">
-        <v>13</v>
-      </c>
-      <c r="CQ3259">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3260" spans="94:95" x14ac:dyDescent="0.2">
-      <c r="CP3260" t="s">
-        <v>14</v>
-      </c>
-      <c r="CQ3260">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>